<commit_message>
Completed re-done report with related data file
</commit_message>
<xml_diff>
--- a/4-17-2017/Experimental Setup (version 1).xlsx
+++ b/4-17-2017/Experimental Setup (version 1).xlsx
@@ -360,7 +360,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1058,11 +1057,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="125088992"/>
-        <c:axId val="125089552"/>
+        <c:axId val="118515984"/>
+        <c:axId val="45558256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="125088992"/>
+        <c:axId val="118515984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1108,7 +1107,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1175,12 +1173,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125089552"/>
+        <c:crossAx val="45558256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="125089552"/>
+        <c:axId val="45558256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1226,7 +1224,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1293,7 +1290,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="125088992"/>
+        <c:crossAx val="118515984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1307,7 +1304,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1609,11 +1605,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209231680"/>
-        <c:axId val="209232240"/>
+        <c:axId val="200661264"/>
+        <c:axId val="200661824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209231680"/>
+        <c:axId val="200661264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1726,12 +1722,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209232240"/>
+        <c:crossAx val="200661824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209232240"/>
+        <c:axId val="200661824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1844,7 +1840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209231680"/>
+        <c:crossAx val="200661264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1970,7 +1966,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2054,7 +2049,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2166,11 +2160,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209234480"/>
-        <c:axId val="209235040"/>
+        <c:axId val="200664064"/>
+        <c:axId val="200664624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209234480"/>
+        <c:axId val="200664064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2216,7 +2210,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2283,12 +2276,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209235040"/>
+        <c:crossAx val="200664624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209235040"/>
+        <c:axId val="200664624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2334,7 +2327,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2401,7 +2393,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209234480"/>
+        <c:crossAx val="200664064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2415,7 +2407,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2527,7 +2518,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2611,7 +2601,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -2723,11 +2712,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209237280"/>
-        <c:axId val="209543488"/>
+        <c:axId val="201127296"/>
+        <c:axId val="201127856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209237280"/>
+        <c:axId val="201127296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2773,7 +2762,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2840,12 +2828,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209543488"/>
+        <c:crossAx val="201127856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209543488"/>
+        <c:axId val="201127856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2879,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2958,7 +2945,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209237280"/>
+        <c:crossAx val="201127296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2972,7 +2959,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3084,7 +3070,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3168,7 +3153,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -3280,11 +3264,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209545728"/>
-        <c:axId val="209546288"/>
+        <c:axId val="201189808"/>
+        <c:axId val="201190368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209545728"/>
+        <c:axId val="201189808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3330,7 +3314,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3397,12 +3380,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209546288"/>
+        <c:crossAx val="201190368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209546288"/>
+        <c:axId val="201190368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3448,7 +3431,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3515,7 +3497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209545728"/>
+        <c:crossAx val="201189808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3529,7 +3511,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3641,7 +3622,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3842,11 +3822,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209548528"/>
-        <c:axId val="209549088"/>
+        <c:axId val="201192608"/>
+        <c:axId val="201193168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209548528"/>
+        <c:axId val="201192608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3892,7 +3872,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3959,12 +3938,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209549088"/>
+        <c:crossAx val="201193168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209549088"/>
+        <c:axId val="201193168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4010,7 +3989,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4077,7 +4055,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209548528"/>
+        <c:crossAx val="201192608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4091,7 +4069,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4203,7 +4180,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4404,11 +4380,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209948912"/>
-        <c:axId val="209949472"/>
+        <c:axId val="201195408"/>
+        <c:axId val="201195968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209948912"/>
+        <c:axId val="201195408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4454,7 +4430,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4521,12 +4496,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209949472"/>
+        <c:crossAx val="201195968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209949472"/>
+        <c:axId val="201195968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4572,7 +4547,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4639,7 +4613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209948912"/>
+        <c:crossAx val="201195408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4653,7 +4627,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4765,7 +4738,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4865,7 +4837,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -4965,11 +4936,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209950592"/>
-        <c:axId val="209951152"/>
+        <c:axId val="201275264"/>
+        <c:axId val="201275824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209950592"/>
+        <c:axId val="201275264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5015,7 +4986,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5082,12 +5052,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209951152"/>
+        <c:crossAx val="201275824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209951152"/>
+        <c:axId val="201275824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5133,7 +5103,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5200,7 +5169,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209950592"/>
+        <c:crossAx val="201275264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5214,7 +5183,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5326,7 +5294,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5413,7 +5380,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -5513,11 +5479,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209953392"/>
-        <c:axId val="209953952"/>
+        <c:axId val="201278064"/>
+        <c:axId val="201278624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209953392"/>
+        <c:axId val="201278064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5563,7 +5529,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5630,12 +5595,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209953952"/>
+        <c:crossAx val="201278624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="209953952"/>
+        <c:axId val="201278624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5681,7 +5646,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5748,7 +5712,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209953392"/>
+        <c:crossAx val="201278064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5762,7 +5726,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5874,7 +5837,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5961,7 +5923,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -6055,11 +6016,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="209956192"/>
-        <c:axId val="210268272"/>
+        <c:axId val="201280864"/>
+        <c:axId val="201281424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="209956192"/>
+        <c:axId val="201280864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6105,7 +6066,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6172,12 +6132,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210268272"/>
+        <c:crossAx val="201281424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210268272"/>
+        <c:axId val="201281424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6223,7 +6183,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6290,7 +6249,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="209956192"/>
+        <c:crossAx val="201280864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6304,7 +6263,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6416,7 +6374,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6503,7 +6460,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -6591,11 +6547,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210270512"/>
-        <c:axId val="210271072"/>
+        <c:axId val="201835488"/>
+        <c:axId val="201836048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210270512"/>
+        <c:axId val="201835488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6641,7 +6597,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6708,12 +6663,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210271072"/>
+        <c:crossAx val="201836048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210271072"/>
+        <c:axId val="201836048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6759,7 +6714,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6826,7 +6780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210270512"/>
+        <c:crossAx val="201835488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6840,7 +6794,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8835,11 +8788,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="126851552"/>
-        <c:axId val="127024592"/>
+        <c:axId val="118022752"/>
+        <c:axId val="119606320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="126851552"/>
+        <c:axId val="118022752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8952,12 +8905,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127024592"/>
+        <c:crossAx val="119606320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127024592"/>
+        <c:axId val="119606320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9070,7 +9023,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126851552"/>
+        <c:crossAx val="118022752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9196,7 +9149,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9283,7 +9235,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -9359,11 +9310,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210273312"/>
-        <c:axId val="210273872"/>
+        <c:axId val="201838288"/>
+        <c:axId val="201838848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210273312"/>
+        <c:axId val="201838288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9409,7 +9360,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9476,12 +9426,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210273872"/>
+        <c:crossAx val="201838848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210273872"/>
+        <c:axId val="201838848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9527,7 +9477,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9594,7 +9543,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210273312"/>
+        <c:crossAx val="201838288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9608,7 +9557,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9720,7 +9668,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9807,7 +9754,6 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -9883,11 +9829,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210812688"/>
-        <c:axId val="210813248"/>
+        <c:axId val="201841088"/>
+        <c:axId val="201841648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210812688"/>
+        <c:axId val="201841088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9933,7 +9879,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10000,12 +9945,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210813248"/>
+        <c:crossAx val="201841648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210813248"/>
+        <c:axId val="201841648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10051,7 +9996,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10118,7 +10062,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210812688"/>
+        <c:crossAx val="201841088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10132,7 +10076,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11108,11 +11051,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210819968"/>
-        <c:axId val="210584624"/>
+        <c:axId val="201627472"/>
+        <c:axId val="201628032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210819968"/>
+        <c:axId val="201627472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11225,12 +11168,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210584624"/>
+        <c:crossAx val="201628032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210584624"/>
+        <c:axId val="201628032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11343,7 +11286,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210819968"/>
+        <c:crossAx val="201627472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11658,11 +11601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210587424"/>
-        <c:axId val="210587984"/>
+        <c:axId val="200307280"/>
+        <c:axId val="200307840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210587424"/>
+        <c:axId val="200307280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11774,12 +11717,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210587984"/>
+        <c:crossAx val="200307840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210587984"/>
+        <c:axId val="200307840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11891,7 +11834,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210587424"/>
+        <c:crossAx val="200307280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12206,11 +12149,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="210590224"/>
-        <c:axId val="210590784"/>
+        <c:axId val="200310080"/>
+        <c:axId val="200310640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="210590224"/>
+        <c:axId val="200310080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12322,12 +12265,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210590784"/>
+        <c:crossAx val="200310640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="210590784"/>
+        <c:axId val="200310640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12439,7 +12382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="210590224"/>
+        <c:crossAx val="200310080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12754,11 +12697,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="211148816"/>
-        <c:axId val="211149376"/>
+        <c:axId val="200312880"/>
+        <c:axId val="200313440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="211148816"/>
+        <c:axId val="200312880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12870,12 +12813,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211149376"/>
+        <c:crossAx val="200313440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="211149376"/>
+        <c:axId val="200313440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12987,7 +12930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211148816"/>
+        <c:crossAx val="200312880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13302,11 +13245,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="211151616"/>
-        <c:axId val="211152176"/>
+        <c:axId val="202102864"/>
+        <c:axId val="202103424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="211151616"/>
+        <c:axId val="202102864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13418,12 +13361,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211152176"/>
+        <c:crossAx val="202103424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="211152176"/>
+        <c:axId val="202103424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13535,7 +13478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211151616"/>
+        <c:crossAx val="202102864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13850,11 +13793,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="211154416"/>
-        <c:axId val="211154976"/>
+        <c:axId val="202105664"/>
+        <c:axId val="202106224"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="211154416"/>
+        <c:axId val="202105664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13966,12 +13909,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211154976"/>
+        <c:crossAx val="202106224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="211154976"/>
+        <c:axId val="202106224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14083,7 +14026,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211154416"/>
+        <c:crossAx val="202105664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14386,11 +14329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="211466784"/>
-        <c:axId val="211467344"/>
+        <c:axId val="202108464"/>
+        <c:axId val="202572832"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="211466784"/>
+        <c:axId val="202108464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14502,12 +14445,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211467344"/>
+        <c:crossAx val="202572832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="211467344"/>
+        <c:axId val="202572832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14619,7 +14562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211466784"/>
+        <c:crossAx val="202108464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14917,11 +14860,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="211469584"/>
-        <c:axId val="211470144"/>
+        <c:axId val="202575072"/>
+        <c:axId val="202575632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="211469584"/>
+        <c:axId val="202575072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15034,12 +14977,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211470144"/>
+        <c:crossAx val="202575632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="211470144"/>
+        <c:axId val="202575632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15152,7 +15095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211469584"/>
+        <c:crossAx val="202575072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15397,63 +15340,49 @@
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -15495,7 +15424,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -15642,63 +15570,49 @@
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -15740,7 +15654,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -15887,63 +15800,49 @@
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -15985,7 +15884,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -16132,63 +16030,49 @@
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -16230,7 +16114,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -16356,45 +16239,35 @@
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -16571,27 +16444,21 @@
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -16633,7 +16500,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -16735,9 +16601,7 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -16798,7 +16662,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -16863,8 +16726,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="281226096"/>
-        <c:axId val="281226656"/>
+        <c:axId val="199886336"/>
+        <c:axId val="199886880"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -17027,7 +16890,7 @@
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$C$5,'average rpm from log data'!$C$22,'average rpm from log data'!$C$39,'average rpm from log data'!$C$56,'average rpm from log data'!$C$73,'average rpm from log data'!$C$90,'average rpm from log data'!$C$107,'average rpm from log data'!$C$124)</c15:sqref>
@@ -17066,7 +16929,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$D$5,'average rpm from log data'!$D$22,'average rpm from log data'!$D$39,'average rpm from log data'!$D$56,'average rpm from log data'!$D$73,'average rpm from log data'!$D$90,'average rpm from log data'!$D$107,'average rpm from log data'!$D$124)</c15:sqref>
@@ -17104,7 +16967,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17156,7 +17019,7 @@
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$C$7,'average rpm from log data'!$C$24,'average rpm from log data'!$C$41,'average rpm from log data'!$C$58,'average rpm from log data'!$C$75,'average rpm from log data'!$C$92,'average rpm from log data'!$C$109,'average rpm from log data'!$C$126)</c15:sqref>
@@ -17195,7 +17058,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$D$7,'average rpm from log data'!$D$24,'average rpm from log data'!$D$41,'average rpm from log data'!$D$58,'average rpm from log data'!$D$75,'average rpm from log data'!$D$92,'average rpm from log data'!$D$109,'average rpm from log data'!$D$126)</c15:sqref>
@@ -17233,7 +17096,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17291,7 +17154,7 @@
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$C$9,'average rpm from log data'!$C$26,'average rpm from log data'!$C$43,'average rpm from log data'!$C$60,'average rpm from log data'!$C$77,'average rpm from log data'!$C$94,'average rpm from log data'!$C$111,'average rpm from log data'!$C$128)</c15:sqref>
@@ -17330,7 +17193,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$D$9,'average rpm from log data'!$D$26,'average rpm from log data'!$D$43,'average rpm from log data'!$D$60,'average rpm from log data'!$D$77,'average rpm from log data'!$D$94,'average rpm from log data'!$D$111,'average rpm from log data'!$D$128)</c15:sqref>
@@ -17368,7 +17231,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17426,7 +17289,7 @@
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$C$11,'average rpm from log data'!$C$28,'average rpm from log data'!$C$45,'average rpm from log data'!$C$62,'average rpm from log data'!$C$79,'average rpm from log data'!$C$96,'average rpm from log data'!$C$113,'average rpm from log data'!$C$130)</c15:sqref>
@@ -17465,7 +17328,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$D$11,'average rpm from log data'!$D$28,'average rpm from log data'!$D$45,'average rpm from log data'!$D$62,'average rpm from log data'!$D$79,'average rpm from log data'!$D$96,'average rpm from log data'!$D$113,'average rpm from log data'!$D$130)</c15:sqref>
@@ -17503,7 +17366,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17577,7 +17440,7 @@
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$C$47,'average rpm from log data'!$C$64,'average rpm from log data'!$C$81,'average rpm from log data'!$C$98,'average rpm from log data'!$C$115,'average rpm from log data'!$C$132)</c15:sqref>
@@ -17610,7 +17473,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$D$47,'average rpm from log data'!$D$64,'average rpm from log data'!$D$81,'average rpm from log data'!$D$98,'average rpm from log data'!$D$115,'average rpm from log data'!$D$132)</c15:sqref>
@@ -17642,7 +17505,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17703,7 +17566,7 @@
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$C$66,'average rpm from log data'!$C$83,'average rpm from log data'!$C$100,'average rpm from log data'!$C$117,'average rpm from log data'!$C$134)</c15:sqref>
@@ -17733,7 +17596,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$D$66,'average rpm from log data'!$D$83,'average rpm from log data'!$D$100,'average rpm from log data'!$D$117,'average rpm from log data'!$D$134)</c15:sqref>
@@ -17762,7 +17625,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17823,7 +17686,7 @@
                 </c:trendline>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$C$119,'average rpm from log data'!$C$136)</c15:sqref>
@@ -17844,7 +17707,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>('average rpm from log data'!$D$119,'average rpm from log data'!$D$136)</c15:sqref>
@@ -17864,7 +17727,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000F-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17875,7 +17738,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="281226096"/>
+        <c:axId val="199886336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17988,12 +17851,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281226656"/>
+        <c:crossAx val="199886880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="281226656"/>
+        <c:axId val="199886880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18106,7 +17969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281226096"/>
+        <c:crossAx val="199886336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -19132,11 +18995,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="211837712"/>
-        <c:axId val="211838272"/>
+        <c:axId val="202987200"/>
+        <c:axId val="202987760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="211837712"/>
+        <c:axId val="202987200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19249,12 +19112,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211838272"/>
+        <c:crossAx val="202987760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="211838272"/>
+        <c:axId val="202987760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19367,7 +19230,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211837712"/>
+        <c:crossAx val="202987200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20357,11 +20220,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="211957552"/>
-        <c:axId val="211958112"/>
+        <c:axId val="203072992"/>
+        <c:axId val="203073552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="211957552"/>
+        <c:axId val="203072992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20474,12 +20337,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211958112"/>
+        <c:crossAx val="203073552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="211958112"/>
+        <c:axId val="203073552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20592,7 +20455,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="211957552"/>
+        <c:crossAx val="203072992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20762,63 +20625,49 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -20871,7 +20720,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -20991,63 +20839,49 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -21100,7 +20934,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -21224,63 +21057,49 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -21432,54 +21251,42 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -21507,9 +21314,7 @@
               <c:idx val="7"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -21541,7 +21346,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -21665,36 +21469,28 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -21722,9 +21518,7 @@
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -21756,7 +21550,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -21864,27 +21657,21 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -21937,7 +21724,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -22083,7 +21869,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -22198,7 +21983,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -22243,11 +22027,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="212057312"/>
-        <c:axId val="212057872"/>
+        <c:axId val="203359392"/>
+        <c:axId val="203359952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="212057312"/>
+        <c:axId val="203359392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22340,12 +22124,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212057872"/>
+        <c:crossAx val="203359952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="212057872"/>
+        <c:axId val="203359952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22438,7 +22222,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="212057312"/>
+        <c:crossAx val="203359392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -22601,63 +22385,49 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -22720,7 +22490,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -22846,63 +22615,49 @@
               <c:idx val="0"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -22965,7 +22720,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -23066,8 +22820,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="238865648"/>
-        <c:axId val="238866208"/>
+        <c:axId val="119520720"/>
+        <c:axId val="119520160"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -23307,7 +23061,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23436,7 +23190,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23571,7 +23325,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23706,7 +23460,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23845,7 +23599,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23965,7 +23719,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -24067,7 +23821,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000F-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -24078,7 +23832,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="238865648"/>
+        <c:axId val="119520720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24191,12 +23945,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238866208"/>
+        <c:crossAx val="119520160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="238866208"/>
+        <c:axId val="119520160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24309,7 +24063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="238865648"/>
+        <c:crossAx val="119520720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -24593,11 +24347,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="127026832"/>
-        <c:axId val="127027392"/>
+        <c:axId val="119796384"/>
+        <c:axId val="119795824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127026832"/>
+        <c:axId val="119796384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24710,12 +24464,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127027392"/>
+        <c:crossAx val="119795824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127027392"/>
+        <c:axId val="119795824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24828,7 +24582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127026832"/>
+        <c:crossAx val="119796384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -25150,11 +24904,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="127029632"/>
-        <c:axId val="127030192"/>
+        <c:axId val="3337200"/>
+        <c:axId val="3336640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="127029632"/>
+        <c:axId val="3337200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25267,12 +25021,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127030192"/>
+        <c:crossAx val="3336640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="127030192"/>
+        <c:axId val="3336640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25385,7 +25139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="127029632"/>
+        <c:crossAx val="3337200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -25707,11 +25461,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="126463232"/>
-        <c:axId val="126462672"/>
+        <c:axId val="3334400"/>
+        <c:axId val="119145600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="126463232"/>
+        <c:axId val="3334400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25824,12 +25578,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126462672"/>
+        <c:crossAx val="119145600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126462672"/>
+        <c:axId val="119145600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25942,7 +25696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126463232"/>
+        <c:crossAx val="3334400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -26258,11 +26012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="126460432"/>
-        <c:axId val="126459872"/>
+        <c:axId val="119147840"/>
+        <c:axId val="119148400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="126460432"/>
+        <c:axId val="119147840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26375,12 +26129,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126459872"/>
+        <c:crossAx val="119148400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126459872"/>
+        <c:axId val="119148400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26493,7 +26247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126460432"/>
+        <c:crossAx val="119147840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -26814,11 +26568,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="126457632"/>
-        <c:axId val="126457072"/>
+        <c:axId val="201061184"/>
+        <c:axId val="201061744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="126457632"/>
+        <c:axId val="201061184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26931,12 +26685,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126457072"/>
+        <c:crossAx val="201061744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="126457072"/>
+        <c:axId val="201061744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27049,7 +26803,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="126457632"/>
+        <c:crossAx val="201061184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -50571,8 +50325,8 @@
   <dimension ref="A1:J137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R52" sqref="R52"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E137" sqref="A1:E137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -53045,7 +52799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A49"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
@@ -54632,9 +54386,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:E1048576"/>
+      <selection pane="bottomLeft" activeCell="E73" sqref="A1:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Poster updated to repo
</commit_message>
<xml_diff>
--- a/4-17-2017/Experimental Setup (version 1).xlsx
+++ b/4-17-2017/Experimental Setup (version 1).xlsx
@@ -1057,11 +1057,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118515984"/>
-        <c:axId val="45558256"/>
+        <c:axId val="250331568"/>
+        <c:axId val="250331008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118515984"/>
+        <c:axId val="250331568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1173,12 +1173,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45558256"/>
+        <c:crossAx val="250331008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45558256"/>
+        <c:axId val="250331008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1290,7 +1290,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118515984"/>
+        <c:crossAx val="250331568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1605,11 +1605,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="200661264"/>
-        <c:axId val="200661824"/>
+        <c:axId val="315860304"/>
+        <c:axId val="257063600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="200661264"/>
+        <c:axId val="315860304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1722,12 +1722,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200661824"/>
+        <c:crossAx val="257063600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="200661824"/>
+        <c:axId val="257063600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1840,7 +1840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200661264"/>
+        <c:crossAx val="315860304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2160,11 +2160,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="200664064"/>
-        <c:axId val="200664624"/>
+        <c:axId val="329504464"/>
+        <c:axId val="329505024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="200664064"/>
+        <c:axId val="329504464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2276,12 +2276,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200664624"/>
+        <c:crossAx val="329505024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="200664624"/>
+        <c:axId val="329505024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2393,7 +2393,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200664064"/>
+        <c:crossAx val="329504464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2712,11 +2712,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201127296"/>
-        <c:axId val="201127856"/>
+        <c:axId val="329507264"/>
+        <c:axId val="329507824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201127296"/>
+        <c:axId val="329507264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2828,12 +2828,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201127856"/>
+        <c:crossAx val="329507824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201127856"/>
+        <c:axId val="329507824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2945,7 +2945,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201127296"/>
+        <c:crossAx val="329507264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3264,11 +3264,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201189808"/>
-        <c:axId val="201190368"/>
+        <c:axId val="329510064"/>
+        <c:axId val="329519168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201189808"/>
+        <c:axId val="329510064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3380,12 +3380,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201190368"/>
+        <c:crossAx val="329519168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201190368"/>
+        <c:axId val="329519168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3497,7 +3497,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201189808"/>
+        <c:crossAx val="329510064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3822,11 +3822,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201192608"/>
-        <c:axId val="201193168"/>
+        <c:axId val="329521408"/>
+        <c:axId val="329521968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201192608"/>
+        <c:axId val="329521408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3938,12 +3938,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201193168"/>
+        <c:crossAx val="329521968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201193168"/>
+        <c:axId val="329521968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4055,7 +4055,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201192608"/>
+        <c:crossAx val="329521408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4380,11 +4380,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201195408"/>
-        <c:axId val="201195968"/>
+        <c:axId val="329524208"/>
+        <c:axId val="329524768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201195408"/>
+        <c:axId val="329524208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4496,12 +4496,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201195968"/>
+        <c:crossAx val="329524768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201195968"/>
+        <c:axId val="329524768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4613,7 +4613,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201195408"/>
+        <c:crossAx val="329524208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4936,11 +4936,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201275264"/>
-        <c:axId val="201275824"/>
+        <c:axId val="329525888"/>
+        <c:axId val="329526448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201275264"/>
+        <c:axId val="329525888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5052,12 +5052,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201275824"/>
+        <c:crossAx val="329526448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201275824"/>
+        <c:axId val="329526448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5169,7 +5169,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201275264"/>
+        <c:crossAx val="329525888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5479,11 +5479,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201278064"/>
-        <c:axId val="201278624"/>
+        <c:axId val="252778480"/>
+        <c:axId val="252779040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201278064"/>
+        <c:axId val="252778480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5595,12 +5595,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201278624"/>
+        <c:crossAx val="252779040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201278624"/>
+        <c:axId val="252779040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5712,7 +5712,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201278064"/>
+        <c:crossAx val="252778480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6016,11 +6016,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201280864"/>
-        <c:axId val="201281424"/>
+        <c:axId val="252781280"/>
+        <c:axId val="252781840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201280864"/>
+        <c:axId val="252781280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6132,12 +6132,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201281424"/>
+        <c:crossAx val="252781840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201281424"/>
+        <c:axId val="252781840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6249,7 +6249,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201280864"/>
+        <c:crossAx val="252781280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6547,11 +6547,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201835488"/>
-        <c:axId val="201836048"/>
+        <c:axId val="252784080"/>
+        <c:axId val="307224640"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201835488"/>
+        <c:axId val="252784080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6663,12 +6663,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201836048"/>
+        <c:crossAx val="307224640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201836048"/>
+        <c:axId val="307224640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6780,7 +6780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201835488"/>
+        <c:crossAx val="252784080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8788,11 +8788,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="118022752"/>
-        <c:axId val="119606320"/>
+        <c:axId val="313013248"/>
+        <c:axId val="253041936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118022752"/>
+        <c:axId val="313013248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8905,12 +8905,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119606320"/>
+        <c:crossAx val="253041936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119606320"/>
+        <c:axId val="253041936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9023,7 +9023,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="118022752"/>
+        <c:crossAx val="313013248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9310,11 +9310,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201838288"/>
-        <c:axId val="201838848"/>
+        <c:axId val="307226880"/>
+        <c:axId val="307227440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201838288"/>
+        <c:axId val="307226880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9426,12 +9426,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201838848"/>
+        <c:crossAx val="307227440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201838848"/>
+        <c:axId val="307227440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9543,7 +9543,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201838288"/>
+        <c:crossAx val="307226880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9829,11 +9829,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201841088"/>
-        <c:axId val="201841648"/>
+        <c:axId val="307229680"/>
+        <c:axId val="307230240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201841088"/>
+        <c:axId val="307229680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9945,12 +9945,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201841648"/>
+        <c:crossAx val="307230240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201841648"/>
+        <c:axId val="307230240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10062,7 +10062,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201841088"/>
+        <c:crossAx val="307229680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11051,11 +11051,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201627472"/>
-        <c:axId val="201628032"/>
+        <c:axId val="250452368"/>
+        <c:axId val="250452928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201627472"/>
+        <c:axId val="250452368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11168,12 +11168,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201628032"/>
+        <c:crossAx val="250452928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201628032"/>
+        <c:axId val="250452928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11286,7 +11286,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201627472"/>
+        <c:crossAx val="250452368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11601,11 +11601,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="200307280"/>
-        <c:axId val="200307840"/>
+        <c:axId val="250455728"/>
+        <c:axId val="250456288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="200307280"/>
+        <c:axId val="250455728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11717,12 +11717,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200307840"/>
+        <c:crossAx val="250456288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="200307840"/>
+        <c:axId val="250456288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11834,7 +11834,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200307280"/>
+        <c:crossAx val="250455728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12149,11 +12149,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="200310080"/>
-        <c:axId val="200310640"/>
+        <c:axId val="250458528"/>
+        <c:axId val="250459088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="200310080"/>
+        <c:axId val="250458528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12265,12 +12265,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200310640"/>
+        <c:crossAx val="250459088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="200310640"/>
+        <c:axId val="250459088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12382,7 +12382,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200310080"/>
+        <c:crossAx val="250458528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12697,11 +12697,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="200312880"/>
-        <c:axId val="200313440"/>
+        <c:axId val="250461328"/>
+        <c:axId val="250461888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="200312880"/>
+        <c:axId val="250461328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12813,12 +12813,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200313440"/>
+        <c:crossAx val="250461888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="200313440"/>
+        <c:axId val="250461888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12930,7 +12930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200312880"/>
+        <c:crossAx val="250461328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13245,11 +13245,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202102864"/>
-        <c:axId val="202103424"/>
+        <c:axId val="321801104"/>
+        <c:axId val="321801664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="202102864"/>
+        <c:axId val="321801104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13361,12 +13361,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202103424"/>
+        <c:crossAx val="321801664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202103424"/>
+        <c:axId val="321801664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13478,7 +13478,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202102864"/>
+        <c:crossAx val="321801104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13793,11 +13793,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202105664"/>
-        <c:axId val="202106224"/>
+        <c:axId val="321803904"/>
+        <c:axId val="321804464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="202105664"/>
+        <c:axId val="321803904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13909,12 +13909,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202106224"/>
+        <c:crossAx val="321804464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202106224"/>
+        <c:axId val="321804464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14026,7 +14026,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202105664"/>
+        <c:crossAx val="321803904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14329,11 +14329,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202108464"/>
-        <c:axId val="202572832"/>
+        <c:axId val="321806704"/>
+        <c:axId val="321807264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="202108464"/>
+        <c:axId val="321806704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14445,12 +14445,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202572832"/>
+        <c:crossAx val="321807264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202572832"/>
+        <c:axId val="321807264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14562,7 +14562,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202108464"/>
+        <c:crossAx val="321806704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -14860,11 +14860,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202575072"/>
-        <c:axId val="202575632"/>
+        <c:axId val="321809504"/>
+        <c:axId val="321810064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="202575072"/>
+        <c:axId val="321809504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14977,12 +14977,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202575632"/>
+        <c:crossAx val="321810064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202575632"/>
+        <c:axId val="321810064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15095,7 +15095,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202575072"/>
+        <c:crossAx val="321809504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15215,7 +15215,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Torque vs Supply Current at high constant values of Motor Speed</a:t>
+              <a:t>Torque vs Supply Current at high constant values of Motor Speed at 91.5V</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -16726,8 +16726,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="199886336"/>
-        <c:axId val="199886880"/>
+        <c:axId val="257061920"/>
+        <c:axId val="257062480"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -16967,7 +16967,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17096,7 +17096,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17231,7 +17231,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17366,7 +17366,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17505,7 +17505,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17625,7 +17625,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17727,7 +17727,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000F-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -17738,7 +17738,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="199886336"/>
+        <c:axId val="257061920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17851,12 +17851,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199886880"/>
+        <c:crossAx val="257062480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="199886880"/>
+        <c:axId val="257062480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17969,7 +17969,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="199886336"/>
+        <c:crossAx val="257061920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18995,11 +18995,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202987200"/>
-        <c:axId val="202987760"/>
+        <c:axId val="321816784"/>
+        <c:axId val="251682160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="202987200"/>
+        <c:axId val="321816784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19112,12 +19112,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202987760"/>
+        <c:crossAx val="251682160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="202987760"/>
+        <c:axId val="251682160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -19230,7 +19230,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202987200"/>
+        <c:crossAx val="321816784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20220,11 +20220,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203072992"/>
-        <c:axId val="203073552"/>
+        <c:axId val="251689440"/>
+        <c:axId val="179709856"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203072992"/>
+        <c:axId val="251689440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20337,12 +20337,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203073552"/>
+        <c:crossAx val="179709856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203073552"/>
+        <c:axId val="179709856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20455,7 +20455,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203072992"/>
+        <c:crossAx val="251689440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -20571,7 +20571,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Motor Speed vs Supply Current at constant values of Torque</a:t>
+              <a:t>Motor Speed vs Supply Current at constant values of Torque at 91.5V</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -22027,11 +22027,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203359392"/>
-        <c:axId val="203359952"/>
+        <c:axId val="179716576"/>
+        <c:axId val="179717136"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203359392"/>
+        <c:axId val="179716576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22124,12 +22124,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203359952"/>
+        <c:crossAx val="179717136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203359952"/>
+        <c:axId val="179717136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22222,7 +22222,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203359392"/>
+        <c:crossAx val="179716576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -22310,7 +22310,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Torque vs Supply Current at low constant values of Motor Speed</a:t>
+              <a:t>Torque vs Supply Current at low constant values of Motor Speed at 91.5V</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -22820,8 +22820,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119520720"/>
-        <c:axId val="119520160"/>
+        <c:axId val="315294400"/>
+        <c:axId val="315294960"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredScatterSeries>
@@ -23061,7 +23061,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23190,7 +23190,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23325,7 +23325,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23460,7 +23460,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23599,7 +23599,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23719,7 +23719,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000D-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23821,7 +23821,7 @@
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart" xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000F-A427-4EEF-BD7B-4CCDAB5A042B}"/>
                   </c:ext>
@@ -23832,7 +23832,7 @@
         </c:extLst>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119520720"/>
+        <c:axId val="315294400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23945,12 +23945,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119520160"/>
+        <c:crossAx val="315294960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119520160"/>
+        <c:axId val="315294960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24063,7 +24063,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119520720"/>
+        <c:crossAx val="315294400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -24347,11 +24347,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119796384"/>
-        <c:axId val="119795824"/>
+        <c:axId val="315297200"/>
+        <c:axId val="315297760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119796384"/>
+        <c:axId val="315297200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24464,12 +24464,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119795824"/>
+        <c:crossAx val="315297760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119795824"/>
+        <c:axId val="315297760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -24582,7 +24582,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119796384"/>
+        <c:crossAx val="315297200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -24904,11 +24904,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="3337200"/>
-        <c:axId val="3336640"/>
+        <c:axId val="176276160"/>
+        <c:axId val="176273360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3337200"/>
+        <c:axId val="176276160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25021,12 +25021,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3336640"/>
+        <c:crossAx val="176273360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="3336640"/>
+        <c:axId val="176273360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25139,7 +25139,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3337200"/>
+        <c:crossAx val="176276160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -25461,11 +25461,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="3334400"/>
-        <c:axId val="119145600"/>
+        <c:axId val="176276720"/>
+        <c:axId val="176271120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="3334400"/>
+        <c:axId val="176276720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25578,12 +25578,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119145600"/>
+        <c:crossAx val="176271120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119145600"/>
+        <c:axId val="176271120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25696,7 +25696,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3334400"/>
+        <c:crossAx val="176276720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -26012,11 +26012,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="119147840"/>
-        <c:axId val="119148400"/>
+        <c:axId val="315854144"/>
+        <c:axId val="315854704"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="119147840"/>
+        <c:axId val="315854144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26129,12 +26129,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119148400"/>
+        <c:crossAx val="315854704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="119148400"/>
+        <c:axId val="315854704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26247,7 +26247,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119147840"/>
+        <c:crossAx val="315854144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -26568,11 +26568,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="201061184"/>
-        <c:axId val="201061744"/>
+        <c:axId val="315857504"/>
+        <c:axId val="315858064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="201061184"/>
+        <c:axId val="315857504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26685,12 +26685,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201061744"/>
+        <c:crossAx val="315858064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="201061744"/>
+        <c:axId val="315858064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26803,7 +26803,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201061184"/>
+        <c:crossAx val="315857504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -50325,8 +50325,8 @@
   <dimension ref="A1:J137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E137" sqref="A1:E137"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T55" sqref="T55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -56120,7 +56120,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A48" zoomScaleNormal="100" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="J83" sqref="J83"/>
+      <selection activeCell="S65" sqref="S65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>